<commit_message>
Excel Modified - Conflict Testing
</commit_message>
<xml_diff>
--- a/src/test/resources/Amazon.xlsx
+++ b/src/test/resources/Amazon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UB217ZA\Downloads\excel-version-control\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93E09E9-4140-4791-AA8E-258BA4FC9A89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C317EF-EBE6-4C06-8652-9EEEDC7B91FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -513,7 +513,7 @@
     <t>twotabsearchtextbox</t>
   </si>
   <si>
-    <t>home_1</t>
+    <t>amazon_login</t>
   </si>
 </sst>
 </file>
@@ -892,7 +892,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>